<commit_message>
Fix error for time series in step_2
</commit_message>
<xml_diff>
--- a/PRO1/step_2/time_series_example/res_bus/vm_pu.xlsx
+++ b/PRO1/step_2/time_series_example/res_bus/vm_pu.xlsx
@@ -442,61 +442,61 @@
         <v>1.03</v>
       </c>
       <c r="C2">
-        <v>0.9972901753822303</v>
+        <v>1.022289158843633</v>
       </c>
       <c r="D2">
-        <v>0.9877384920205977</v>
+        <v>1.017227016238946</v>
       </c>
       <c r="E2">
-        <v>0.9722441381192682</v>
+        <v>1.008798052176311</v>
       </c>
       <c r="F2">
-        <v>0.9713735063161697</v>
+        <v>1.008355365585052</v>
       </c>
       <c r="G2">
-        <v>0.970777596797892</v>
+        <v>1.008053228998541</v>
       </c>
       <c r="H2">
-        <v>0.9700801700342763</v>
+        <v>1.007703459746382</v>
       </c>
       <c r="I2">
-        <v>0.9699202188083061</v>
+        <v>1.007462140347889</v>
       </c>
       <c r="J2">
-        <v>0.9699875801559662</v>
+        <v>1.007499084881931</v>
       </c>
       <c r="K2">
-        <v>0.969594627887546</v>
+        <v>1.007258570533565</v>
       </c>
       <c r="L2">
-        <v>0.9690273796608185</v>
+        <v>1.006958548742034</v>
       </c>
       <c r="M2">
-        <v>0.9689375188854444</v>
+        <v>1.00691360838677</v>
       </c>
       <c r="N2">
-        <v>1.001410718218441</v>
+        <v>1.022735154818722</v>
       </c>
       <c r="O2">
-        <v>0.9997068799377746</v>
+        <v>1.021435645688297</v>
       </c>
       <c r="P2">
-        <v>0.9987174581058191</v>
+        <v>1.020682097350532</v>
       </c>
       <c r="Q2">
-        <v>0.969965227945113</v>
+        <v>1.007475868262984</v>
       </c>
       <c r="R2">
-        <v>0.9996838428809299</v>
+        <v>1.02141210791787</v>
       </c>
       <c r="S2">
-        <v>0.9707552263820419</v>
+        <v>1.008029999610002</v>
       </c>
       <c r="T2">
-        <v>0.9689151908720083</v>
+        <v>1.006890405259433</v>
       </c>
       <c r="U2">
-        <v>0.972221733908712</v>
+        <v>1.008774805624207</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -507,61 +507,61 @@
         <v>1.03</v>
       </c>
       <c r="C3">
-        <v>0.9986362103804298</v>
+        <v>1.022655332694385</v>
       </c>
       <c r="D3">
-        <v>0.9895187342846201</v>
+        <v>1.017840348719568</v>
       </c>
       <c r="E3">
-        <v>0.9747031994276153</v>
+        <v>1.009794673876673</v>
       </c>
       <c r="F3">
-        <v>0.9738694658290185</v>
+        <v>1.009371101343759</v>
       </c>
       <c r="G3">
-        <v>0.9732988806246001</v>
+        <v>1.009082074132424</v>
       </c>
       <c r="H3">
-        <v>0.9726314200779831</v>
+        <v>1.008747805230651</v>
       </c>
       <c r="I3">
-        <v>0.9724814963831446</v>
+        <v>1.008519198126675</v>
       </c>
       <c r="J3">
-        <v>0.9725442189313989</v>
+        <v>1.008552845717094</v>
       </c>
       <c r="K3">
-        <v>0.9721677102998025</v>
+        <v>1.008322297147755</v>
       </c>
       <c r="L3">
-        <v>0.9716243603012932</v>
+        <v>1.008035002965413</v>
       </c>
       <c r="M3">
-        <v>0.9715383740062387</v>
+        <v>1.007992064561174</v>
       </c>
       <c r="N3">
-        <v>1.002524184070991</v>
+        <v>1.023023629411535</v>
       </c>
       <c r="O3">
-        <v>1.000887402362707</v>
+        <v>1.021774508229384</v>
       </c>
       <c r="P3">
-        <v>0.9999365453085443</v>
+        <v>1.021049812177786</v>
       </c>
       <c r="Q3">
-        <v>0.972521807805791</v>
+        <v>1.00852960481548</v>
       </c>
       <c r="R3">
-        <v>1.000864338102124</v>
+        <v>1.021750962650272</v>
       </c>
       <c r="S3">
-        <v>0.9732764521087108</v>
+        <v>1.00905882103537</v>
       </c>
       <c r="T3">
-        <v>0.9715159860591319</v>
+        <v>1.007968836582096</v>
       </c>
       <c r="U3">
-        <v>0.9746807385508685</v>
+        <v>1.009771404358605</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -572,61 +572,61 @@
         <v>1.03</v>
       </c>
       <c r="C4">
-        <v>1.000021328506111</v>
+        <v>1.023031750231346</v>
       </c>
       <c r="D4">
-        <v>0.991350209152595</v>
+        <v>1.018471576111606</v>
       </c>
       <c r="E4">
-        <v>0.9772325097445393</v>
+        <v>1.010821184499963</v>
       </c>
       <c r="F4">
-        <v>0.9764367106198487</v>
+        <v>1.010417329248058</v>
       </c>
       <c r="G4">
-        <v>0.9758921604070564</v>
+        <v>1.010141825224188</v>
       </c>
       <c r="H4">
-        <v>0.9752555058257896</v>
+        <v>1.009823545788094</v>
       </c>
       <c r="I4">
-        <v>0.9751158805280782</v>
+        <v>1.009608047384511</v>
       </c>
       <c r="J4">
-        <v>0.9751738343348062</v>
+        <v>1.009638294103649</v>
       </c>
       <c r="K4">
-        <v>0.9748142286448793</v>
+        <v>1.009418025208367</v>
       </c>
       <c r="L4">
-        <v>0.9742954438460979</v>
+        <v>1.009143859390712</v>
       </c>
       <c r="M4">
-        <v>0.9742134401477196</v>
+        <v>1.009102985982179</v>
       </c>
       <c r="N4">
-        <v>1.003671487913512</v>
+        <v>1.023320613389119</v>
       </c>
       <c r="O4">
-        <v>1.002103853819911</v>
+        <v>1.02212354562585</v>
       </c>
       <c r="P4">
-        <v>1.001192764047729</v>
+        <v>1.021428655481585</v>
       </c>
       <c r="Q4">
-        <v>0.9751513626128372</v>
+        <v>1.009615028189167</v>
       </c>
       <c r="R4">
-        <v>1.002080761527651</v>
+        <v>1.022099992003586</v>
       </c>
       <c r="S4">
-        <v>0.9758696721321169</v>
+        <v>1.010118547706431</v>
       </c>
       <c r="T4">
-        <v>0.974190990556893</v>
+        <v>1.009079732403237</v>
       </c>
       <c r="U4">
-        <v>0.9772099905828421</v>
+        <v>1.010797891327178</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -637,61 +637,61 @@
         <v>1.03</v>
       </c>
       <c r="C5">
-        <v>1.000028267954923</v>
+        <v>1.023033635094677</v>
       </c>
       <c r="D5">
-        <v>0.9913593836921579</v>
+        <v>1.018474738794024</v>
       </c>
       <c r="E5">
-        <v>0.9772451786892096</v>
+        <v>1.010826329774751</v>
       </c>
       <c r="F5">
-        <v>0.9764495695277176</v>
+        <v>1.010422573430317</v>
       </c>
       <c r="G5">
-        <v>0.975905149688099</v>
+        <v>1.010147137242824</v>
       </c>
       <c r="H5">
-        <v>0.9752686493681556</v>
+        <v>1.009828938014265</v>
       </c>
       <c r="I5">
-        <v>0.9751290756140168</v>
+        <v>1.009613505355474</v>
       </c>
       <c r="J5">
-        <v>0.9751870055413338</v>
+        <v>1.009643735015185</v>
       </c>
       <c r="K5">
-        <v>0.9748274844893235</v>
+        <v>1.009423517684097</v>
       </c>
       <c r="L5">
-        <v>0.9743088226941872</v>
+        <v>1.009149417719711</v>
       </c>
       <c r="M5">
-        <v>0.9742268389375519</v>
+        <v>1.009108554669439</v>
       </c>
       <c r="N5">
-        <v>1.003677239748487</v>
+        <v>1.023322101619865</v>
       </c>
       <c r="O5">
-        <v>1.002109952452541</v>
+        <v>1.022125295162709</v>
       </c>
       <c r="P5">
-        <v>1.00119906212596</v>
+        <v>1.021430554642843</v>
       </c>
       <c r="Q5">
-        <v>0.97516453351585</v>
+        <v>1.009620468975325</v>
       </c>
       <c r="R5">
-        <v>1.002086860019745</v>
+        <v>1.022101741500129</v>
       </c>
       <c r="S5">
-        <v>0.975882661113837</v>
+        <v>1.010123859602657</v>
       </c>
       <c r="T5">
-        <v>0.9742043890379665</v>
+        <v>1.009085300962173</v>
       </c>
       <c r="U5">
-        <v>0.9772226592355718</v>
+        <v>1.010803036483399</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -702,61 +702,61 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.000914867588316</v>
+        <v>1.023274359897387</v>
       </c>
       <c r="D6">
-        <v>0.992531450429468</v>
+        <v>1.018878818130062</v>
       </c>
       <c r="E6">
-        <v>0.9788635575649791</v>
+        <v>1.011483888133937</v>
       </c>
       <c r="F6">
-        <v>0.9780922114046455</v>
+        <v>1.011092778416864</v>
       </c>
       <c r="G6">
-        <v>0.977564443333263</v>
+        <v>1.010826016026064</v>
       </c>
       <c r="H6">
-        <v>0.9769476456224842</v>
+        <v>1.010518072377817</v>
       </c>
       <c r="I6">
-        <v>0.9768146530448285</v>
+        <v>1.010311045050431</v>
       </c>
       <c r="J6">
-        <v>0.9768695330498532</v>
+        <v>1.010339093462655</v>
       </c>
       <c r="K6">
-        <v>0.9765208218379801</v>
+        <v>1.010125469165176</v>
       </c>
       <c r="L6">
-        <v>0.9760178697874166</v>
+        <v>1.009859789218191</v>
       </c>
       <c r="M6">
-        <v>0.9759384329414672</v>
+        <v>1.009820250579889</v>
       </c>
       <c r="N6">
-        <v>1.004412418302985</v>
+        <v>1.023512263747025</v>
       </c>
       <c r="O6">
-        <v>1.002889468635563</v>
+        <v>1.022348884620628</v>
       </c>
       <c r="P6">
-        <v>1.002004077154457</v>
+        <v>1.021673284649903</v>
       </c>
       <c r="Q6">
-        <v>0.9768470222525228</v>
+        <v>1.010315811399085</v>
       </c>
       <c r="R6">
-        <v>1.002866358239743</v>
+        <v>1.022325325805695</v>
       </c>
       <c r="S6">
-        <v>0.9775419165225511</v>
+        <v>1.010802722741942</v>
       </c>
       <c r="T6">
-        <v>0.9759159436002319</v>
+        <v>1.009796980472437</v>
       </c>
       <c r="U6">
-        <v>0.9788410008177236</v>
+        <v>1.011460579689934</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -767,61 +767,61 @@
         <v>1.03</v>
       </c>
       <c r="C7">
-        <v>1.000223088644751</v>
+        <v>1.02308654635407</v>
       </c>
       <c r="D7">
-        <v>0.9916169486129623</v>
+        <v>1.018563528611868</v>
       </c>
       <c r="E7">
-        <v>0.9776008399696585</v>
+        <v>1.01097078813476</v>
       </c>
       <c r="F7">
-        <v>0.9768105635583022</v>
+        <v>1.010569809034488</v>
       </c>
       <c r="G7">
-        <v>0.9762698036197655</v>
+        <v>1.010296277640188</v>
       </c>
       <c r="H7">
-        <v>0.975637633788958</v>
+        <v>1.009980330575598</v>
       </c>
       <c r="I7">
-        <v>0.9754995068858862</v>
+        <v>1.009766743927788</v>
       </c>
       <c r="J7">
-        <v>0.975556766460796</v>
+        <v>1.009796494573498</v>
       </c>
       <c r="K7">
-        <v>0.9751996213851313</v>
+        <v>1.009577725117882</v>
       </c>
       <c r="L7">
-        <v>0.9746844125728664</v>
+        <v>1.009305474251786</v>
       </c>
       <c r="M7">
-        <v>0.9746029886246805</v>
+        <v>1.009264902051886</v>
       </c>
       <c r="N7">
-        <v>1.003838734176344</v>
+        <v>1.023363883467172</v>
       </c>
       <c r="O7">
-        <v>1.002281184481541</v>
+        <v>1.022174415087835</v>
       </c>
       <c r="P7">
-        <v>1.001375894312373</v>
+        <v>1.021483876365552</v>
       </c>
       <c r="Q7">
-        <v>0.9755342859146112</v>
+        <v>1.009773225013475</v>
       </c>
       <c r="R7">
-        <v>1.002258088102906</v>
+        <v>1.022150860293345</v>
       </c>
       <c r="S7">
-        <v>0.9762473066424868</v>
+        <v>1.010272996563257</v>
       </c>
       <c r="T7">
-        <v>0.9745805300571726</v>
+        <v>1.00924164474178</v>
       </c>
       <c r="U7">
-        <v>0.9775783123202293</v>
+        <v>1.010947491514537</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -832,61 +832,61 @@
         <v>1.03</v>
       </c>
       <c r="C8">
-        <v>0.9985508245369584</v>
+        <v>1.022632115302205</v>
       </c>
       <c r="D8">
-        <v>0.9894058175954611</v>
+        <v>1.017801439266656</v>
       </c>
       <c r="E8">
-        <v>0.9745472416792441</v>
+        <v>1.009731425804202</v>
       </c>
       <c r="F8">
-        <v>0.9737111684463516</v>
+        <v>1.009306639396018</v>
       </c>
       <c r="G8">
-        <v>0.9731389774982291</v>
+        <v>1.009016779645823</v>
       </c>
       <c r="H8">
-        <v>0.9724696169120071</v>
+        <v>1.008681526366058</v>
       </c>
       <c r="I8">
-        <v>0.9723190577006737</v>
+        <v>1.008452112079125</v>
       </c>
       <c r="J8">
-        <v>0.9723820743754207</v>
+        <v>1.008485969044896</v>
       </c>
       <c r="K8">
-        <v>0.9720045231604946</v>
+        <v>1.008254787596981</v>
       </c>
       <c r="L8">
-        <v>0.9714596579477067</v>
+        <v>1.007966685149228</v>
       </c>
       <c r="M8">
-        <v>0.9713734260002533</v>
+        <v>1.007923619611054</v>
       </c>
       <c r="N8">
-        <v>1.002453508224538</v>
+        <v>1.023005326083875</v>
       </c>
       <c r="O8">
-        <v>1.000812468674793</v>
+        <v>1.021753002778662</v>
       </c>
       <c r="P8">
-        <v>0.9998591629035514</v>
+        <v>1.02102647318297</v>
       </c>
       <c r="Q8">
-        <v>0.9723596669862417</v>
+        <v>1.008462729684375</v>
       </c>
       <c r="R8">
-        <v>1.000789406140968</v>
+        <v>1.021729457695119</v>
       </c>
       <c r="S8">
-        <v>0.9731165526671173</v>
+        <v>1.008993528053403</v>
       </c>
       <c r="T8">
-        <v>0.9713510418541774</v>
+        <v>1.007900393209208</v>
       </c>
       <c r="U8">
-        <v>0.9745247843963583</v>
+        <v>1.009708157743611</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -897,61 +897,61 @@
         <v>1.03</v>
       </c>
       <c r="C9">
-        <v>0.9939089825861223</v>
+        <v>1.021367808284789</v>
       </c>
       <c r="D9">
-        <v>0.9832645937986839</v>
+        <v>1.015686830480329</v>
       </c>
       <c r="E9">
-        <v>0.9660620515891098</v>
+        <v>1.006298724947466</v>
       </c>
       <c r="F9">
-        <v>0.9650985798809205</v>
+        <v>1.005808228780087</v>
       </c>
       <c r="G9">
-        <v>0.9644389492921673</v>
+        <v>1.005473302386472</v>
       </c>
       <c r="H9">
-        <v>0.9636661163628544</v>
+        <v>1.005084762186626</v>
       </c>
       <c r="I9">
-        <v>0.9634808885720269</v>
+        <v>1.004811625714154</v>
       </c>
       <c r="J9">
-        <v>0.9635599230865473</v>
+        <v>1.004856817326992</v>
       </c>
       <c r="K9">
-        <v>0.9631255860613008</v>
+        <v>1.004591373203736</v>
       </c>
       <c r="L9">
-        <v>0.9624981892419439</v>
+        <v>1.004259512269839</v>
       </c>
       <c r="M9">
-        <v>0.9623985768582565</v>
+        <v>1.004209563910557</v>
       </c>
       <c r="N9">
-        <v>0.9986201860671033</v>
+        <v>1.0220111543317</v>
       </c>
       <c r="O9">
-        <v>0.996748514908223</v>
+        <v>1.020585927059005</v>
       </c>
       <c r="P9">
-        <v>0.9956625707288366</v>
+        <v>1.019760392012305</v>
       </c>
       <c r="Q9">
-        <v>0.9635377189933592</v>
+        <v>1.004833661595959</v>
       </c>
       <c r="R9">
-        <v>0.9967255460233829</v>
+        <v>1.020562408869334</v>
       </c>
       <c r="S9">
-        <v>0.964416724942865</v>
+        <v>1.005450132449275</v>
       </c>
       <c r="T9">
-        <v>0.962376399526912</v>
+        <v>1.00418642309471</v>
       </c>
       <c r="U9">
-        <v>0.9660397898373446</v>
+        <v>1.006275535989387</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -962,61 +962,61 @@
         <v>1.03</v>
       </c>
       <c r="C10">
-        <v>0.977294160382346</v>
+        <v>1.016816200112428</v>
       </c>
       <c r="D10">
-        <v>0.9612346156534075</v>
+        <v>1.008137291022508</v>
       </c>
       <c r="E10">
-        <v>0.9355687675011428</v>
+        <v>0.9941133976715693</v>
       </c>
       <c r="F10">
-        <v>0.9341455607484727</v>
+        <v>0.9933922580389386</v>
       </c>
       <c r="G10">
-        <v>0.9331703376582441</v>
+        <v>0.9928991545724419</v>
       </c>
       <c r="H10">
-        <v>0.9320239263308159</v>
+        <v>0.992323569837805</v>
       </c>
       <c r="I10">
-        <v>0.9317125119718371</v>
+        <v>0.9918965305620858</v>
       </c>
       <c r="J10">
-        <v>0.9318493825624278</v>
+        <v>0.991981518002619</v>
       </c>
       <c r="K10">
-        <v>0.9312098741846546</v>
+        <v>0.9915957543347296</v>
       </c>
       <c r="L10">
-        <v>0.9302842287478458</v>
+        <v>0.991110215807829</v>
       </c>
       <c r="M10">
-        <v>0.9301362612311664</v>
+        <v>0.9910360961680742</v>
       </c>
       <c r="N10">
-        <v>0.9850484949528675</v>
+        <v>1.018472088620866</v>
       </c>
       <c r="O10">
-        <v>0.9823650073110161</v>
+        <v>1.016446826037</v>
       </c>
       <c r="P10">
-        <v>0.9808121732392364</v>
+        <v>1.015277705718913</v>
       </c>
       <c r="Q10">
-        <v>0.9318279092009564</v>
+        <v>0.9919586589675564</v>
       </c>
       <c r="R10">
-        <v>0.9823423698770128</v>
+        <v>1.016423403227992</v>
       </c>
       <c r="S10">
-        <v>0.9331488338569327</v>
+        <v>0.9928762743915357</v>
       </c>
       <c r="T10">
-        <v>0.9301148273465402</v>
+        <v>0.9910132589191344</v>
       </c>
       <c r="U10">
-        <v>0.9355472084308664</v>
+        <v>0.9940904895098737</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1027,61 +1027,61 @@
         <v>1.03</v>
       </c>
       <c r="C11">
-        <v>0.9619333220416297</v>
+        <v>1.012591242428508</v>
       </c>
       <c r="D11">
-        <v>0.9407882127348668</v>
+        <v>1.001207020264033</v>
       </c>
       <c r="E11">
-        <v>0.907177229907861</v>
+        <v>0.9830148435403838</v>
       </c>
       <c r="F11">
-        <v>0.905322831103369</v>
+        <v>0.9820869389960781</v>
       </c>
       <c r="G11">
-        <v>0.9040515259878814</v>
+        <v>0.9814520458858355</v>
       </c>
       <c r="H11">
-        <v>0.9025544482235447</v>
+        <v>0.9807087736521346</v>
       </c>
       <c r="I11">
-        <v>0.902123018866442</v>
+        <v>0.9801431694951593</v>
       </c>
       <c r="J11">
-        <v>0.9023141857049828</v>
+        <v>0.980263847115714</v>
       </c>
       <c r="K11">
-        <v>0.9014818564821838</v>
+        <v>0.9797701432958862</v>
       </c>
       <c r="L11">
-        <v>0.9002758300562224</v>
+        <v>0.9791467226605524</v>
       </c>
       <c r="M11">
-        <v>0.9000824018882909</v>
+        <v>0.9790509173137909</v>
       </c>
       <c r="N11">
-        <v>0.9727266526643082</v>
+        <v>1.015240559909141</v>
       </c>
       <c r="O11">
-        <v>0.9693122690085463</v>
+        <v>1.01268673211814</v>
       </c>
       <c r="P11">
-        <v>0.9673390746518531</v>
+        <v>1.011214947200763</v>
       </c>
       <c r="Q11">
-        <v>0.9022933929470189</v>
+        <v>0.98024125810045</v>
       </c>
       <c r="R11">
-        <v>0.9692899323593834</v>
+        <v>1.012663395956027</v>
       </c>
       <c r="S11">
-        <v>0.9040306931949758</v>
+        <v>0.9814294294899431</v>
       </c>
       <c r="T11">
-        <v>0.9000616605591326</v>
+        <v>0.9790283562490529</v>
       </c>
       <c r="U11">
-        <v>0.9071563250868234</v>
+        <v>0.982992191131677</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1092,61 +1092,61 @@
         <v>1.03</v>
       </c>
       <c r="C12">
-        <v>0.9353286375716811</v>
+        <v>1.005307355699312</v>
       </c>
       <c r="D12">
-        <v>0.9051446806340581</v>
+        <v>0.9894018886197531</v>
       </c>
       <c r="E12">
-        <v>0.8574196211679821</v>
+        <v>0.9642743755764234</v>
       </c>
       <c r="F12">
-        <v>0.8548002877657092</v>
+        <v>0.9630037695817428</v>
       </c>
       <c r="G12">
-        <v>0.8530035094996444</v>
+        <v>0.9621338924684013</v>
       </c>
       <c r="H12">
-        <v>0.8508835916599183</v>
+        <v>0.9611126705478537</v>
       </c>
       <c r="I12">
-        <v>0.8502347438350967</v>
+        <v>0.9603160992398404</v>
       </c>
       <c r="J12">
-        <v>0.8505223685802967</v>
+        <v>0.9604959617406394</v>
       </c>
       <c r="K12">
-        <v>0.8493469238686517</v>
+        <v>0.9598231827693738</v>
       </c>
       <c r="L12">
-        <v>0.847641740667301</v>
+        <v>0.9589709777215992</v>
       </c>
       <c r="M12">
-        <v>0.8473673733611456</v>
+        <v>0.9588391924520447</v>
       </c>
       <c r="N12">
-        <v>0.9519760210071886</v>
+        <v>1.009783730223958</v>
       </c>
       <c r="O12">
-        <v>0.9473432974888021</v>
+        <v>1.006374188348661</v>
       </c>
       <c r="P12">
-        <v>0.9446693785484542</v>
+        <v>1.00441240075274</v>
       </c>
       <c r="Q12">
-        <v>0.8505027693032015</v>
+        <v>0.9604738282527988</v>
       </c>
       <c r="R12">
-        <v>0.9473214670884769</v>
+        <v>1.006350997651618</v>
       </c>
       <c r="S12">
-        <v>0.8529838530476057</v>
+        <v>0.9621117212363939</v>
       </c>
       <c r="T12">
-        <v>0.8473478467871655</v>
+        <v>0.9588170971424835</v>
       </c>
       <c r="U12">
-        <v>0.8573998629518987</v>
+        <v>0.9642521550195268</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1157,61 +1157,61 @@
         <v>1.03</v>
       </c>
       <c r="C13">
-        <v>0.9126413533340926</v>
+        <v>0.9992125271268099</v>
       </c>
       <c r="D13">
-        <v>0.8744473575192483</v>
+        <v>0.9796358140182047</v>
       </c>
       <c r="E13">
-        <v>0.8142222590007084</v>
+        <v>0.948904377502179</v>
       </c>
       <c r="F13">
-        <v>0.8109267431689245</v>
+        <v>0.9473580896617564</v>
       </c>
       <c r="G13">
-        <v>0.8086651868026086</v>
+        <v>0.9462992057976216</v>
       </c>
       <c r="H13">
-        <v>0.8059937666231543</v>
+        <v>0.9450543745720796</v>
       </c>
       <c r="I13">
-        <v>0.8051471381436692</v>
+        <v>0.944070757924949</v>
       </c>
       <c r="J13">
-        <v>0.8055201964276865</v>
+        <v>0.9442982588853431</v>
       </c>
       <c r="K13">
-        <v>0.8040401460142448</v>
+        <v>0.943481261178403</v>
       </c>
       <c r="L13">
-        <v>0.801891542594341</v>
+        <v>0.9424447707422442</v>
       </c>
       <c r="M13">
-        <v>0.8015452660333942</v>
+        <v>0.9422840063176972</v>
       </c>
       <c r="N13">
-        <v>0.9349798132045728</v>
+        <v>1.005324253443278</v>
       </c>
       <c r="O13">
-        <v>0.9293602066422884</v>
+        <v>1.001245654958081</v>
       </c>
       <c r="P13">
-        <v>0.9261186644265043</v>
+        <v>0.9989007425601724</v>
       </c>
       <c r="Q13">
-        <v>0.8055016341721613</v>
+        <v>0.9442764986543131</v>
       </c>
       <c r="R13">
-        <v>0.9293387906409177</v>
+        <v>1.001222582441994</v>
       </c>
       <c r="S13">
-        <v>0.8086465520745181</v>
+        <v>0.9462773994571483</v>
       </c>
       <c r="T13">
-        <v>0.8015267953754153</v>
+        <v>0.9422622925027236</v>
       </c>
       <c r="U13">
-        <v>0.814203496216494</v>
+        <v>0.9488825111286203</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1222,61 +1222,61 @@
         <v>1.03</v>
       </c>
       <c r="C14">
-        <v>0.9104523071903119</v>
+        <v>0.9986335088522035</v>
       </c>
       <c r="D14">
-        <v>0.8714673454339197</v>
+        <v>0.9787124861276002</v>
       </c>
       <c r="E14">
-        <v>0.8100082817070896</v>
+        <v>0.9474567188065393</v>
       </c>
       <c r="F14">
-        <v>0.8066460872250381</v>
+        <v>0.9458846939276121</v>
       </c>
       <c r="G14">
-        <v>0.804338683368704</v>
+        <v>0.9448081659073029</v>
       </c>
       <c r="H14">
-        <v>0.8016128265724511</v>
+        <v>0.9435424582466517</v>
       </c>
       <c r="I14">
-        <v>0.8007463741133046</v>
+        <v>0.9425413201813846</v>
       </c>
       <c r="J14">
-        <v>0.8011278665939083</v>
+        <v>0.9427732698509765</v>
       </c>
       <c r="K14">
-        <v>0.7996177043408017</v>
+        <v>0.9419428003678</v>
       </c>
       <c r="L14">
-        <v>0.797425250175805</v>
+        <v>0.940889093877081</v>
       </c>
       <c r="M14">
-        <v>0.7970718619086483</v>
+        <v>0.9407256223282664</v>
       </c>
       <c r="N14">
-        <v>0.9333789452217712</v>
+        <v>1.004905526178585</v>
       </c>
       <c r="O14">
-        <v>0.9276668715757512</v>
+        <v>1.000765377201033</v>
       </c>
       <c r="P14">
-        <v>0.9243721442861792</v>
+        <v>0.9983852185726788</v>
       </c>
       <c r="Q14">
-        <v>0.8011094055544036</v>
+        <v>0.942751544761506</v>
       </c>
       <c r="R14">
-        <v>0.9276454945952748</v>
+        <v>1.000742315752375</v>
       </c>
       <c r="S14">
-        <v>0.804320148339743</v>
+        <v>0.9447863939260718</v>
       </c>
       <c r="T14">
-        <v>0.7970534943349508</v>
+        <v>0.9407039444243994</v>
       </c>
       <c r="U14">
-        <v>0.8099896160289731</v>
+        <v>0.9474348857925544</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1287,61 +1287,61 @@
         <v>1.03</v>
       </c>
       <c r="C15">
-        <v>0.9122355974903252</v>
+        <v>0.9991050602169709</v>
       </c>
       <c r="D15">
-        <v>0.8738952544989456</v>
+        <v>0.9794643883350141</v>
       </c>
       <c r="E15">
-        <v>0.8134418386132896</v>
+        <v>0.9486355365505522</v>
       </c>
       <c r="F15">
-        <v>0.8101339843824195</v>
+        <v>0.9470844662886124</v>
       </c>
       <c r="G15">
-        <v>0.8078639444925867</v>
+        <v>0.9460223037970633</v>
       </c>
       <c r="H15">
-        <v>0.8051824519646303</v>
+        <v>0.9447735933509078</v>
       </c>
       <c r="I15">
-        <v>0.8043321597947414</v>
+        <v>0.9437867216786893</v>
       </c>
       <c r="J15">
-        <v>0.8047067786287428</v>
+        <v>0.9440150492754052</v>
       </c>
       <c r="K15">
-        <v>0.803221157304952</v>
+        <v>0.9431955483648091</v>
       </c>
       <c r="L15">
-        <v>0.8010644414107111</v>
+        <v>0.9421558590176562</v>
       </c>
       <c r="M15">
-        <v>0.8007168491765323</v>
+        <v>0.9419945915813173</v>
       </c>
       <c r="N15">
-        <v>0.9346825269768803</v>
+        <v>1.005246472696669</v>
       </c>
       <c r="O15">
-        <v>0.9290457427805838</v>
+        <v>1.001156425026896</v>
       </c>
       <c r="P15">
-        <v>0.9257943203730988</v>
+        <v>0.9988049563799382</v>
       </c>
       <c r="Q15">
-        <v>0.8046882351174638</v>
+        <v>0.9439932955706042</v>
       </c>
       <c r="R15">
-        <v>0.929024334025659</v>
+        <v>1.001133354567006</v>
       </c>
       <c r="S15">
-        <v>0.807845328228173</v>
+        <v>0.9460005038374675</v>
       </c>
       <c r="T15">
-        <v>0.8006983976084352</v>
+        <v>0.9419728844355624</v>
       </c>
       <c r="U15">
-        <v>0.8134230938129356</v>
+        <v>0.9486136763721137</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1352,61 +1352,61 @@
         <v>1.03</v>
       </c>
       <c r="C16">
-        <v>0.9122890425092536</v>
+        <v>0.9991192118468063</v>
       </c>
       <c r="D16">
-        <v>0.8739679827258184</v>
+        <v>0.9794869608645338</v>
       </c>
       <c r="E16">
-        <v>0.8135446505948375</v>
+        <v>0.9486709344942311</v>
       </c>
       <c r="F16">
-        <v>0.8102384220808536</v>
+        <v>0.9471204938527673</v>
       </c>
       <c r="G16">
-        <v>0.80796949999223</v>
+        <v>0.9460587630022119</v>
       </c>
       <c r="H16">
-        <v>0.8052893346238824</v>
+        <v>0.9448105632676265</v>
       </c>
       <c r="I16">
-        <v>0.8044395253022947</v>
+        <v>0.9438241201497827</v>
       </c>
       <c r="J16">
-        <v>0.8048139385135337</v>
+        <v>0.9440523389168516</v>
       </c>
       <c r="K16">
-        <v>0.803329051244481</v>
+        <v>0.9432331675633966</v>
       </c>
       <c r="L16">
-        <v>0.8011734043018592</v>
+        <v>0.9421938993666775</v>
       </c>
       <c r="M16">
-        <v>0.8008259854293848</v>
+        <v>0.9420326981539675</v>
       </c>
       <c r="N16">
-        <v>0.9347216704358825</v>
+        <v>1.00525671347437</v>
       </c>
       <c r="O16">
-        <v>0.9290871478440931</v>
+        <v>1.001168172813538</v>
       </c>
       <c r="P16">
-        <v>0.9258370262613878</v>
+        <v>0.9988175671387021</v>
       </c>
       <c r="Q16">
-        <v>0.8047953925328826</v>
+        <v>0.9440305843527549</v>
       </c>
       <c r="R16">
-        <v>0.9290657381350378</v>
+        <v>1.001145102082935</v>
       </c>
       <c r="S16">
-        <v>0.8079508812954149</v>
+        <v>0.9460369622024571</v>
       </c>
       <c r="T16">
-        <v>0.8008075313463725</v>
+        <v>0.9420109901300919</v>
       </c>
       <c r="U16">
-        <v>0.8135259034253033</v>
+        <v>0.9486490735000889</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1417,61 +1417,61 @@
         <v>1.03</v>
       </c>
       <c r="C17">
-        <v>0.9125209632011567</v>
+        <v>0.9991806344515138</v>
       </c>
       <c r="D17">
-        <v>0.8742835577265511</v>
+        <v>0.9795849378669902</v>
       </c>
       <c r="E17">
-        <v>0.8139907352255116</v>
+        <v>0.9488245869640237</v>
       </c>
       <c r="F17">
-        <v>0.8106915595035672</v>
+        <v>0.9472768795900924</v>
       </c>
       <c r="G17">
-        <v>0.8084274867138641</v>
+        <v>0.9462170225527002</v>
       </c>
       <c r="H17">
-        <v>0.8057530788491383</v>
+        <v>0.9449710398850887</v>
       </c>
       <c r="I17">
-        <v>0.8049053638395152</v>
+        <v>0.9439864571082319</v>
       </c>
       <c r="J17">
-        <v>0.805278885016831</v>
+        <v>0.9442142034326398</v>
       </c>
       <c r="K17">
-        <v>0.8037971821765652</v>
+        <v>0.9433964627217789</v>
       </c>
       <c r="L17">
-        <v>0.8016461724696962</v>
+        <v>0.9423590227819907</v>
       </c>
       <c r="M17">
-        <v>0.8012995056597629</v>
+        <v>0.9421981090529531</v>
       </c>
       <c r="N17">
-        <v>0.9348915805597153</v>
+        <v>1.005301167600768</v>
       </c>
       <c r="O17">
-        <v>0.9292668754900194</v>
+        <v>1.001219170163659</v>
       </c>
       <c r="P17">
-        <v>0.9260224007271913</v>
+        <v>0.9988723113936785</v>
       </c>
       <c r="Q17">
-        <v>0.8052603283220404</v>
+        <v>0.9441924451385678</v>
       </c>
       <c r="R17">
-        <v>0.9292454616393542</v>
+        <v>1.001196098257882</v>
       </c>
       <c r="S17">
-        <v>0.8084088574632897</v>
+        <v>0.946195218106042</v>
       </c>
       <c r="T17">
-        <v>0.8012810406650398</v>
+        <v>0.9421763972173798</v>
       </c>
       <c r="U17">
-        <v>0.813971977776487</v>
+        <v>0.9488027224291429</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1482,61 +1482,61 @@
         <v>1.03</v>
       </c>
       <c r="C18">
-        <v>0.9343421576066683</v>
+        <v>1.005039414811641</v>
       </c>
       <c r="D18">
-        <v>0.9038163521460927</v>
+        <v>0.9889706041878142</v>
       </c>
       <c r="E18">
-        <v>0.8555576789196995</v>
+        <v>0.9635932396230703</v>
       </c>
       <c r="F18">
-        <v>0.8529094541598409</v>
+        <v>0.9623103187172316</v>
       </c>
       <c r="G18">
-        <v>0.8510928227983683</v>
+        <v>0.9614319980843435</v>
       </c>
       <c r="H18">
-        <v>0.8489493596909797</v>
+        <v>0.9604007876873714</v>
       </c>
       <c r="I18">
-        <v>0.848292175435892</v>
+        <v>0.959595885218568</v>
       </c>
       <c r="J18">
-        <v>0.8485834471066804</v>
+        <v>0.9597778752290477</v>
       </c>
       <c r="K18">
-        <v>0.8473950140102501</v>
+        <v>0.9590986571050775</v>
       </c>
       <c r="L18">
-        <v>0.8456709292045793</v>
+        <v>0.9582382246315508</v>
       </c>
       <c r="M18">
-        <v>0.8453934967942596</v>
+        <v>0.9581051455356651</v>
       </c>
       <c r="N18">
-        <v>0.9512226318330945</v>
+        <v>1.009585672469284</v>
       </c>
       <c r="O18">
-        <v>0.9465459581379556</v>
+        <v>1.006145868551085</v>
       </c>
       <c r="P18">
-        <v>0.943846760875338</v>
+        <v>1.004166751998872</v>
       </c>
       <c r="Q18">
-        <v>0.8485638925097261</v>
+        <v>0.9597557582886572</v>
       </c>
       <c r="R18">
-        <v>0.946524146111368</v>
+        <v>1.006122683115399</v>
       </c>
       <c r="S18">
-        <v>0.8510732103758338</v>
+        <v>0.961409843026658</v>
       </c>
       <c r="T18">
-        <v>0.8453740157059187</v>
+        <v>0.9580830671413424</v>
       </c>
       <c r="U18">
-        <v>0.8555379636098623</v>
+        <v>0.9635710347621422</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1547,61 +1547,61 @@
         <v>1.03</v>
       </c>
       <c r="C19">
-        <v>0.9694545709257349</v>
+        <v>1.014660395832781</v>
       </c>
       <c r="D19">
-        <v>0.9508100665337906</v>
+        <v>1.004592570398345</v>
       </c>
       <c r="E19">
-        <v>0.9211053885724043</v>
+        <v>0.9884269094104858</v>
       </c>
       <c r="F19">
-        <v>0.9194629396627478</v>
+        <v>0.9875994550999104</v>
       </c>
       <c r="G19">
-        <v>0.918337182482894</v>
+        <v>0.9870334446715894</v>
       </c>
       <c r="H19">
-        <v>0.9170125085166407</v>
+        <v>0.9863716390691696</v>
       </c>
       <c r="I19">
-        <v>0.9166402836586713</v>
+        <v>0.9858734241294421</v>
       </c>
       <c r="J19">
-        <v>0.916804755047236</v>
+        <v>0.9859767610874683</v>
       </c>
       <c r="K19">
-        <v>0.9160672551526022</v>
+        <v>0.9855355059462356</v>
       </c>
       <c r="L19">
-        <v>0.9149991310534912</v>
+        <v>0.9849790848690502</v>
       </c>
       <c r="M19">
-        <v>0.9148280625139689</v>
+        <v>0.9848938168798265</v>
       </c>
       <c r="N19">
-        <v>0.9787312543702408</v>
+        <v>1.016816918621295</v>
       </c>
       <c r="O19">
-        <v>0.975672331426194</v>
+        <v>1.0145187523213</v>
       </c>
       <c r="P19">
-        <v>0.9739035743352543</v>
+        <v>1.013193363560789</v>
       </c>
       <c r="Q19">
-        <v>0.9167836283713245</v>
+        <v>0.985954040424892</v>
       </c>
       <c r="R19">
-        <v>0.9756498482169522</v>
+        <v>1.01449537394246</v>
       </c>
       <c r="S19">
-        <v>0.9183160204940136</v>
+        <v>0.987010699658996</v>
       </c>
       <c r="T19">
-        <v>0.9148069813885875</v>
+        <v>0.9848711211724125</v>
       </c>
       <c r="U19">
-        <v>0.9210841627935046</v>
+        <v>0.9884041322871535</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1612,61 +1612,61 @@
         <v>1.03</v>
       </c>
       <c r="C20">
-        <v>0.9780755826989778</v>
+        <v>1.017030912286591</v>
       </c>
       <c r="D20">
-        <v>0.9622725757830048</v>
+        <v>1.008491364504199</v>
       </c>
       <c r="E20">
-        <v>0.9370075928254195</v>
+        <v>0.9946825785911125</v>
       </c>
       <c r="F20">
-        <v>0.9356061519461873</v>
+        <v>0.9939721251947979</v>
       </c>
       <c r="G20">
-        <v>0.9346458723900771</v>
+        <v>0.9934863501404043</v>
       </c>
       <c r="H20">
-        <v>0.9335171546709846</v>
+        <v>0.9929194318022335</v>
       </c>
       <c r="I20">
-        <v>0.9332117543595144</v>
+        <v>0.9924995384651304</v>
       </c>
       <c r="J20">
-        <v>0.9333458855102319</v>
+        <v>0.9925826817007029</v>
       </c>
       <c r="K20">
-        <v>0.9327161001300371</v>
+        <v>0.9922024946893024</v>
       </c>
       <c r="L20">
-        <v>0.9318045906434017</v>
+        <v>0.9917240793334874</v>
       </c>
       <c r="M20">
-        <v>0.9316589150500842</v>
+        <v>0.9916510800366151</v>
       </c>
       <c r="N20">
-        <v>0.985681324299656</v>
+        <v>1.018637666273335</v>
       </c>
       <c r="O20">
-        <v>0.9830355300567427</v>
+        <v>1.016639964761899</v>
       </c>
       <c r="P20">
-        <v>0.9815043743525034</v>
+        <v>1.015486626243343</v>
       </c>
       <c r="Q20">
-        <v>0.9333243776636289</v>
+        <v>0.9925598088125376</v>
       </c>
       <c r="R20">
-        <v>0.9830128771713398</v>
+        <v>1.016616537502239</v>
       </c>
       <c r="S20">
-        <v>0.9346243345868216</v>
+        <v>0.9934634564282737</v>
       </c>
       <c r="T20">
-        <v>0.9316374460777106</v>
+        <v>0.9916282286161029</v>
       </c>
       <c r="U20">
-        <v>0.9369860005991236</v>
+        <v>0.9946596573133194</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1677,61 +1677,61 @@
         <v>1.03</v>
       </c>
       <c r="C21">
-        <v>0.9870717572737202</v>
+        <v>1.019498884854459</v>
       </c>
       <c r="D21">
-        <v>0.9742085840411447</v>
+        <v>1.012575472188928</v>
       </c>
       <c r="E21">
-        <v>0.9535379142579465</v>
+        <v>1.001264003159981</v>
       </c>
       <c r="F21">
-        <v>0.9523860002815978</v>
+        <v>1.00067772690385</v>
       </c>
       <c r="G21">
-        <v>0.9515970210149075</v>
+        <v>1.000277112192183</v>
       </c>
       <c r="H21">
-        <v>0.9506710964963522</v>
+        <v>0.9998108984568834</v>
       </c>
       <c r="I21">
-        <v>0.9504343552007153</v>
+        <v>0.9994739335380176</v>
       </c>
       <c r="J21">
-        <v>0.9505370898593712</v>
+        <v>0.9995356492472206</v>
       </c>
       <c r="K21">
-        <v>0.9500187033478775</v>
+        <v>0.9992202503993061</v>
       </c>
       <c r="L21">
-        <v>0.9492691382752334</v>
+        <v>0.9988245872680637</v>
       </c>
       <c r="M21">
-        <v>0.9491497190225276</v>
+        <v>0.9987646035772818</v>
       </c>
       <c r="N21">
-        <v>0.9930062950025174</v>
+        <v>1.020550526167203</v>
       </c>
       <c r="O21">
-        <v>0.9907979349814856</v>
+        <v>1.018874811075854</v>
       </c>
       <c r="P21">
-        <v>0.9895183563982743</v>
+        <v>1.017905845133214</v>
       </c>
       <c r="Q21">
-        <v>0.9505151858618964</v>
+        <v>0.9995126161361819</v>
       </c>
       <c r="R21">
-        <v>0.9907751032206872</v>
+        <v>1.018851332316816</v>
       </c>
       <c r="S21">
-        <v>0.9515750925925792</v>
+        <v>1.000254061995013</v>
       </c>
       <c r="T21">
-        <v>0.949127846995365</v>
+        <v>0.9987415882340747</v>
       </c>
       <c r="U21">
-        <v>0.9535159411100405</v>
+        <v>1.001240930221081</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1742,61 +1742,61 @@
         <v>1.03</v>
       </c>
       <c r="C22">
-        <v>0.9903379090214885</v>
+        <v>1.020392557111709</v>
       </c>
       <c r="D22">
-        <v>0.9785362350552477</v>
+        <v>1.014061154610405</v>
       </c>
       <c r="E22">
-        <v>0.9595246983788731</v>
+        <v>1.003665770495329</v>
       </c>
       <c r="F22">
-        <v>0.9584629256488959</v>
+        <v>1.003125098247971</v>
       </c>
       <c r="G22">
-        <v>0.9577358220259488</v>
+        <v>1.002755759596759</v>
       </c>
       <c r="H22">
-        <v>0.9568831347998061</v>
+        <v>1.00232652894154</v>
       </c>
       <c r="I22">
-        <v>0.9566710702798789</v>
+        <v>1.002019969410845</v>
       </c>
       <c r="J22">
-        <v>0.956762466893317</v>
+        <v>1.002073817098853</v>
       </c>
       <c r="K22">
-        <v>0.9562842936400376</v>
+        <v>1.00178220520208</v>
       </c>
       <c r="L22">
-        <v>0.955593181473722</v>
+        <v>1.001416923170333</v>
       </c>
       <c r="M22">
-        <v>0.9554832391131597</v>
+        <v>1.001361718039357</v>
       </c>
       <c r="N22">
-        <v>0.9956831528935085</v>
+        <v>1.021247641827775</v>
       </c>
       <c r="O22">
-        <v>0.9936351779708082</v>
+        <v>1.019690962606895</v>
       </c>
       <c r="P22">
-        <v>0.9924478392875634</v>
+        <v>1.018790157445786</v>
       </c>
       <c r="Q22">
-        <v>0.956740419439428</v>
+        <v>1.002050725498754</v>
       </c>
       <c r="R22">
-        <v>0.9936122808291175</v>
+        <v>1.019667465040616</v>
       </c>
       <c r="S22">
-        <v>0.9577137521422474</v>
+        <v>1.002732652282105</v>
       </c>
       <c r="T22">
-        <v>0.9554612211375542</v>
+        <v>1.001338642848733</v>
       </c>
       <c r="U22">
-        <v>0.9595025872726424</v>
+        <v>1.003642642210555</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1807,61 +1807,61 @@
         <v>1.03</v>
       </c>
       <c r="C23">
-        <v>0.9914381621724526</v>
+        <v>1.020693252593926</v>
       </c>
       <c r="D23">
-        <v>0.9799934111781675</v>
+        <v>1.014561898369366</v>
       </c>
       <c r="E23">
-        <v>0.9615397773903057</v>
+        <v>1.004476228883589</v>
       </c>
       <c r="F23">
-        <v>0.9605083192236545</v>
+        <v>1.00395098100895</v>
       </c>
       <c r="G23">
-        <v>0.9598020236849574</v>
+        <v>1.003592220788944</v>
       </c>
       <c r="H23">
-        <v>0.9589739637171284</v>
+        <v>1.003175498623109</v>
       </c>
       <c r="I23">
-        <v>0.9587701833832989</v>
+        <v>1.002879216909897</v>
       </c>
       <c r="J23">
-        <v>0.9588577674576804</v>
+        <v>1.002930403593108</v>
       </c>
       <c r="K23">
-        <v>0.9583931145391261</v>
+        <v>1.002646836237869</v>
       </c>
       <c r="L23">
-        <v>0.9577216544113054</v>
+        <v>1.002291828669114</v>
       </c>
       <c r="M23">
-        <v>0.9576148981883276</v>
+        <v>1.002238239591817</v>
       </c>
       <c r="N23">
-        <v>0.9965869249183252</v>
+        <v>1.02148274363565</v>
       </c>
       <c r="O23">
-        <v>0.994593164527749</v>
+        <v>1.019966419816127</v>
       </c>
       <c r="P23">
-        <v>0.9934370053525291</v>
+        <v>1.019088722403998</v>
       </c>
       <c r="Q23">
-        <v>0.9588356717200799</v>
+        <v>1.002907292253991</v>
       </c>
       <c r="R23">
-        <v>0.9945702453103965</v>
+        <v>1.019942915902263</v>
       </c>
       <c r="S23">
-        <v>0.9597799061880946</v>
+        <v>1.003569094199035</v>
       </c>
       <c r="T23">
-        <v>0.9575928310911724</v>
+        <v>1.002215144202796</v>
       </c>
       <c r="U23">
-        <v>0.9615176198489741</v>
+        <v>1.004453081922765</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>1.03</v>
       </c>
       <c r="C24">
-        <v>0.9941441073711104</v>
+        <v>1.021431945517586</v>
       </c>
       <c r="D24">
-        <v>0.9835757983632857</v>
+        <v>1.01579390705414</v>
       </c>
       <c r="E24">
-        <v>0.9664921845930272</v>
+        <v>1.006472329084238</v>
       </c>
       <c r="F24">
-        <v>0.9655351761144836</v>
+        <v>1.005985148077371</v>
       </c>
       <c r="G24">
-        <v>0.9648799817005643</v>
+        <v>1.005652495341633</v>
       </c>
       <c r="H24">
-        <v>0.9641123986865929</v>
+        <v>1.005266643567423</v>
       </c>
       <c r="I24">
-        <v>0.963928932734096</v>
+        <v>1.004995714250284</v>
       </c>
       <c r="J24">
-        <v>0.9640071545311557</v>
+        <v>1.00504033397967</v>
       </c>
       <c r="K24">
-        <v>0.9635756990898372</v>
+        <v>1.004776618630131</v>
       </c>
       <c r="L24">
-        <v>0.962952490475288</v>
+        <v>1.004446965630338</v>
       </c>
       <c r="M24">
-        <v>0.9628535571087118</v>
+        <v>1.004397364556995</v>
       </c>
       <c r="N24">
-        <v>0.9988139352398119</v>
+        <v>1.02206146858564</v>
       </c>
       <c r="O24">
-        <v>0.9969539066559276</v>
+        <v>1.020644944096728</v>
       </c>
       <c r="P24">
-        <v>0.9958746582504338</v>
+        <v>1.019824392304855</v>
       </c>
       <c r="Q24">
-        <v>0.9639849401320507</v>
+        <v>1.005017174019714</v>
       </c>
       <c r="R24">
-        <v>0.9969309330380784</v>
+        <v>1.020621424547079</v>
       </c>
       <c r="S24">
-        <v>0.9648577471881945</v>
+        <v>1.005629321275146</v>
       </c>
       <c r="T24">
-        <v>0.962831369292888</v>
+        <v>1.004374219413506</v>
       </c>
       <c r="U24">
-        <v>0.9664699129293579</v>
+        <v>1.006449136125658</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1937,61 +1937,61 @@
         <v>1.03</v>
       </c>
       <c r="C25">
-        <v>0.9953516277359779</v>
+        <v>1.02176117716206</v>
       </c>
       <c r="D25">
-        <v>0.9851738147499727</v>
+        <v>1.016343881846086</v>
       </c>
       <c r="E25">
-        <v>0.9687006375036022</v>
+        <v>1.007364367842319</v>
       </c>
       <c r="F25">
-        <v>0.9677768047582833</v>
+        <v>1.006894234681052</v>
       </c>
       <c r="G25">
-        <v>0.9671443809547386</v>
+        <v>1.006573274021155</v>
       </c>
       <c r="H25">
-        <v>0.9664037448633458</v>
+        <v>1.006201247149561</v>
       </c>
       <c r="I25">
-        <v>0.9662293173087234</v>
+        <v>1.005941665691835</v>
       </c>
       <c r="J25">
-        <v>0.9663033675893302</v>
+        <v>1.005983344628856</v>
       </c>
       <c r="K25">
-        <v>0.9658867021154064</v>
+        <v>1.00572851902381</v>
       </c>
       <c r="L25">
-        <v>0.9652849895438352</v>
+        <v>1.005410219659989</v>
       </c>
       <c r="M25">
-        <v>0.9651895412383495</v>
+        <v>1.005362404404149</v>
       </c>
       <c r="N25">
-        <v>0.9998096780266327</v>
+        <v>1.022319943301157</v>
       </c>
       <c r="O25">
-        <v>0.9980095085873905</v>
+        <v>1.020948206402851</v>
       </c>
       <c r="P25">
-        <v>0.9969646858064558</v>
+        <v>1.020153300180963</v>
       </c>
       <c r="Q25">
-        <v>0.9662811002767241</v>
+        <v>1.005960162938341</v>
       </c>
       <c r="R25">
-        <v>0.9979865106444498</v>
+        <v>1.020924679864883</v>
       </c>
       <c r="S25">
-        <v>0.9671220942619793</v>
+        <v>1.006550078736419</v>
       </c>
       <c r="T25">
-        <v>0.9651672995925481</v>
+        <v>1.005339237022463</v>
       </c>
       <c r="U25">
-        <v>0.9686783149487603</v>
+        <v>1.007341154327765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>